<commit_message>
Fanalized version with basic exception handeling, documented.
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:S10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -369,70 +369,90 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Achieved Action</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Achieved Drive</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Achieved Knowldge</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Achieved Strategy</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>quest_action</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>quest_description</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>quest_drive</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>quest_hint</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>quest_id</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>quest_is_repeatable</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>quest_knowledge</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>quest_max_repeat</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>quest_strategy</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>user_complete_date</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>user_is_complete</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>user_quest_id</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>user_reflection</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>user_repeat_time</t>
         </is>
@@ -442,54 +462,58 @@
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B2" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" t="inlineStr">
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="inlineStr">
         <is>
           <t>Sign up for the CQ Mobile App!</t>
         </is>
       </c>
-      <c r="D2" t="n">
+      <c r="H2" t="n">
         <v>10</v>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="I2" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="F2" t="n">
-        <v>1</v>
-      </c>
-      <c r="G2" t="inlineStr">
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>001</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="H2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K2" t="b">
-        <v>0</v>
-      </c>
-      <c r="L2" t="b">
+      <c r="L2" t="n">
         <v>0</v>
       </c>
       <c r="M2" t="n">
-        <v>1</v>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="O2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>2019-05-03 19:35:03.012240</t>
+        </is>
+      </c>
+      <c r="P2" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>1</v>
+      </c>
+      <c r="R2" t="inlineStr"/>
+      <c r="S2" t="n">
         <v>1</v>
       </c>
     </row>
@@ -497,54 +521,58 @@
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" t="n">
-        <v>0</v>
-      </c>
-      <c r="C3" t="inlineStr">
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="inlineStr">
         <is>
           <t>Start a list of 3 ways you can gain more enjoyment from your intercultural interactions.</t>
         </is>
       </c>
-      <c r="D3" t="n">
+      <c r="H3" t="n">
         <v>2</v>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="I3" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="F3" t="n">
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>002</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="L3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" t="b">
+        <v>0</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>2019-05-03 19:35:03.012240</t>
+        </is>
+      </c>
+      <c r="P3" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q3" t="n">
         <v>2</v>
       </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="H3" t="n">
-        <v>0</v>
-      </c>
-      <c r="I3" t="n">
-        <v>0</v>
-      </c>
-      <c r="J3" t="n">
-        <v>0</v>
-      </c>
-      <c r="K3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L3" t="b">
-        <v>0</v>
-      </c>
-      <c r="M3" t="n">
-        <v>2</v>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="O3" t="n">
+      <c r="R3" t="inlineStr"/>
+      <c r="S3" t="n">
         <v>1</v>
       </c>
     </row>
@@ -552,111 +580,388 @@
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Start a list of 3 ways you can gain more enjoyment from your intercultural interactions.</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>When you use an idiom, stop and think about how you could say the same thing without using an idiom that people from other cultures might not understand.</t>
+        </is>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>020</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="L4" t="n">
         <v>2</v>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="F4" t="n">
-        <v>2</v>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="H4" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J4" t="n">
-        <v>0</v>
-      </c>
-      <c r="K4" t="b">
-        <v>0</v>
-      </c>
-      <c r="L4" t="b">
-        <v>0</v>
-      </c>
-      <c r="M4" t="n">
+      <c r="M4" t="b">
+        <v>0</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0</v>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>2019-05-03 19:35:03.012240</t>
+        </is>
+      </c>
+      <c r="P4" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q4" t="n">
         <v>3</v>
       </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="O4" t="n">
-        <v>2</v>
+      <c r="R4" t="inlineStr"/>
+      <c r="S4" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B5" t="n">
-        <v>0</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Think of one way your intercultural experience can benefit someone else.</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Refer to a travel  guidebook to learn more about a country.</t>
+        </is>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>015</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="L5" t="n">
         <v>2</v>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="M5" t="b">
+        <v>0</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O5" t="b">
+        <v>0</v>
+      </c>
+      <c r="P5" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>4</v>
+      </c>
+      <c r="R5" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="F5" t="n">
+      <c r="S5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Pay attention to the nonverbal communication during a meeting with diverse participants. Write down what you observed and seek out answers for actions and reactions.</t>
+        </is>
+      </c>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>039</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="L6" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" t="b">
+        <v>0</v>
+      </c>
+      <c r="N6" t="n">
+        <v>3</v>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>2019-05-03 19:35:03.012240</t>
+        </is>
+      </c>
+      <c r="P6" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q6" t="n">
         <v>5</v>
       </c>
-      <c r="G5" t="inlineStr">
+      <c r="R6" t="inlineStr"/>
+      <c r="S6" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Read up on how to behave in a new cultural situation.</t>
+        </is>
+      </c>
+      <c r="H7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>034</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="H5" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" t="n">
-        <v>0</v>
-      </c>
-      <c r="J5" t="n">
-        <v>0</v>
-      </c>
-      <c r="K5" t="b">
-        <v>0</v>
-      </c>
-      <c r="L5" t="b">
-        <v>0</v>
-      </c>
-      <c r="M5" t="n">
+      <c r="L7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" t="b">
+        <v>0</v>
+      </c>
+      <c r="N7" t="n">
+        <v>1</v>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>2019-05-03 19:35:03.012240</t>
+        </is>
+      </c>
+      <c r="P7" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>6</v>
+      </c>
+      <c r="R7" t="inlineStr"/>
+      <c r="S7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="n">
+        <v>1</v>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Greet someone from a different culture  in the culturally appropriate manner for their country.</t>
+        </is>
+      </c>
+      <c r="H8" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>045</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="L8" t="n">
+        <v>0</v>
+      </c>
+      <c r="M8" t="b">
+        <v>0</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0</v>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>2019-05-03 19:35:03.012240</t>
+        </is>
+      </c>
+      <c r="P8" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>7</v>
+      </c>
+      <c r="R8" t="inlineStr"/>
+      <c r="S8" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="n">
+        <v>3</v>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Modify how close or far apart you stand hwen interacting with people from a different culture.</t>
+        </is>
+      </c>
+      <c r="H9" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>043</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="L9" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" t="b">
+        <v>0</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0</v>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>2019-05-03 19:35:03.012240</t>
+        </is>
+      </c>
+      <c r="P9" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>8</v>
+      </c>
+      <c r="R9" t="inlineStr"/>
+      <c r="S9" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="n">
         <v>4</v>
       </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="O5" t="n">
-        <v>1</v>
-      </c>
+      <c r="C10" t="n">
+        <v>12</v>
+      </c>
+      <c r="D10" t="n">
+        <v>2</v>
+      </c>
+      <c r="E10" t="n">
+        <v>4</v>
+      </c>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr"/>
+      <c r="O10" t="inlineStr"/>
+      <c r="P10" t="inlineStr"/>
+      <c r="Q10" t="inlineStr"/>
+      <c r="R10" t="inlineStr"/>
+      <c r="S10" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>